<commit_message>
Test Case and Config updated
</commit_message>
<xml_diff>
--- a/TestData/DriverDetailedRegression.xlsx
+++ b/TestData/DriverDetailedRegression.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Automation Tests" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$36</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -388,6 +388,148 @@
   </si>
   <si>
     <t>Error messages displayed correctly</t>
+  </si>
+  <si>
+    <t>User_TC001</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions.
+1) Launch application and login as global admin.
+2) Click on Users Menu and customize columns
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email).
+5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon Resend Invitation and Check if invitation sent again.</t>
+  </si>
+  <si>
+    <t>Invitation sent successfully</t>
+  </si>
+  <si>
+    <t>User_TC003</t>
+  </si>
+  <si>
+    <t>To validate invite via email for Shipper Admin  based on following conditions
+1) Launch application and login as global admin.
+2) Click on Users Menu.
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email)
+5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Accet email invitation and check if invitation acceted.</t>
+  </si>
+  <si>
+    <t>Invitation accepted successfully</t>
+  </si>
+  <si>
+    <t>User_TC004</t>
+  </si>
+  <si>
+    <t>Validate Forgot password based on following conditions:
+1. Launch application and Set UserName.
+2. Clickon Forgot Password.
+3. Verify email and reset password.
+4. Login with new password.
+5. Check whether user is able to login with new password.</t>
+  </si>
+  <si>
+    <t>Password reset successfully</t>
+  </si>
+  <si>
+    <t>User_TC005</t>
+  </si>
+  <si>
+    <t>Validate delete any  user based on following conditions:
+1. Launch application .
+2. Login as global admin.
+3. Go to Users and search accepted user(except global admin)
+4. Clickon delete.
+5. Check whether deleted user exist.</t>
+  </si>
+  <si>
+    <t>User deleted successfully</t>
+  </si>
+  <si>
+    <t>User_TC006</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions
+1) Launch application and login as global admin.
+2) Click on Users Menu and customize columns
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email).
+5) Select role shipper user.
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon Resend Invitation and Check if invitation sent again.
+9.) CLick on cancel invite and check if invitation cancelled</t>
+  </si>
+  <si>
+    <t>User_TC007</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions
+1) Launch application and login as shipper  admin.
+2) Click on Users Menu and customize columns
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email).
+5) Select role shipper user.
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon Resend Invitation and Check if invitation sent again.
+9.) CLick on cancel invite and check if invitation cancelled</t>
+  </si>
+  <si>
+    <t>User_TC008</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions
+1) Launch application and login as shipper  admin.
+2) Click on Users Menu and customize columns
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email).
+5) Select role shipper admin.
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon Resend Invitation and Check if invitation sent again.
+9.) CLick on cancel invite and check if invitation cancelled</t>
+  </si>
+  <si>
+    <t>User_TC009</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions
+1) Launch application and login as Carrier.
+2) Click on Users Menu and customize columns
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email).
+5) Select role shipper admin.
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon Resend Invitation and Check if invitation sent again.
+9.) CLick on cancel invite and check if invitation cancelled</t>
+  </si>
+  <si>
+    <t>User_TC002</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions
+1) Launch application and login as global admin.
+2) Click on Users Menu.
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email)
+5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
+6) Select any one value from Carrier Drop Down field
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon cancel invitation and check if invitation cancelled.</t>
+  </si>
+  <si>
+    <t>Invitation cancelled successfully</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -776,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,440 +953,584 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="150.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="181.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>72</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>83</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>85</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>87</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="150.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
+    <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F27"/>
+  <autoFilter ref="A1:F36"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Config updated for Chrome Browser
</commit_message>
<xml_diff>
--- a/TestData/DriverDetailedRegression.xlsx
+++ b/TestData/DriverDetailedRegression.xlsx
@@ -1669,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3144,7 +3144,7 @@
         <v>200</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>187</v>
+        <v>228</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>201</v>

</xml_diff>